<commit_message>
Graphs update and more art
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ACD204-816B-4631-8456-563378D83207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7621FD-79D2-4DC4-92E9-60EBDBBE651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="137">
   <si>
     <t>Fecha</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>Bolombolo</t>
+  </si>
+  <si>
+    <t>Fondo de Ciudad</t>
   </si>
 </sst>
 </file>
@@ -3549,7 +3552,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A15:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
@@ -3688,7 +3691,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
@@ -3822,8 +3825,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I107" totalsRowShown="0">
-  <autoFilter ref="A1:I107" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I108" totalsRowShown="0">
+  <autoFilter ref="A1:I108" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4105,10 +4108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6232,6 +6235,25 @@
       </c>
       <c r="H107" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E108" s="1"/>
+      <c r="F108" t="s">
+        <v>7</v>
+      </c>
+      <c r="H108" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV changes, new images and began on Heliophysics
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7621FD-79D2-4DC4-92E9-60EBDBBE651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48232C97-15C7-4816-B846-9701308B7B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="138">
   <si>
     <t>Fecha</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>Fondo de Ciudad</t>
+  </si>
+  <si>
+    <t>Astronauta Muerto</t>
   </si>
 </sst>
 </file>
@@ -3825,8 +3828,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I108" totalsRowShown="0">
-  <autoFilter ref="A1:I108" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I109" totalsRowShown="0">
+  <autoFilter ref="A1:I109" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4108,10 +4111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6254,6 +6257,25 @@
       </c>
       <c r="H108" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>44959</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E109" s="1"/>
+      <c r="F109" t="s">
+        <v>5</v>
+      </c>
+      <c r="H109" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to CV and nodes network
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48232C97-15C7-4816-B846-9701308B7B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7A2795-FC26-4757-80EA-E1BC5C261FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="142">
   <si>
     <t>Fecha</t>
   </si>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>Astronauta Muerto</t>
+  </si>
+  <si>
+    <t>Cascada</t>
+  </si>
+  <si>
+    <t>Barbosa</t>
+  </si>
+  <si>
+    <t>Alimentando Peces</t>
+  </si>
+  <si>
+    <t>Barco Nocturno</t>
   </si>
 </sst>
 </file>
@@ -3828,8 +3840,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I109" totalsRowShown="0">
-  <autoFilter ref="A1:I109" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I112" totalsRowShown="0">
+  <autoFilter ref="A1:I112" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4111,10 +4123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:B109"/>
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6275,6 +6287,63 @@
         <v>5</v>
       </c>
       <c r="H109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>44961</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+      <c r="H110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F111" t="s">
+        <v>5</v>
+      </c>
+      <c r="H111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>44973</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D112" s="7"/>
+      <c r="E112" s="1"/>
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New art and emergencia
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F004582A-A0BE-4FE5-92A3-858ED004B882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413A1993-8AF9-40B8-AC3D-3F976AEF6598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="169">
   <si>
     <t>Fecha</t>
   </si>
@@ -523,6 +523,30 @@
   </si>
   <si>
     <t>Sketchers</t>
+  </si>
+  <si>
+    <t>Juanse</t>
+  </si>
+  <si>
+    <t>Mari Reyes</t>
+  </si>
+  <si>
+    <t>Nader</t>
+  </si>
+  <si>
+    <t>Tom Cobley</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Artem</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>El Poblado</t>
   </si>
 </sst>
 </file>
@@ -584,13 +608,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -606,6 +623,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3897,17 +3921,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I123" totalsRowShown="0">
-  <autoFilter ref="A1:I123" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I124" totalsRowShown="0">
+  <autoFilter ref="A1:I124" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{76608A75-85B8-408D-9369-BCFC9E9D7A8A}" name="Nombre" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DE856492-D85D-466F-A960-54F03A0A74D6}" name="Inspiración" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{8733A214-F4B8-45AB-8117-68932FC446F0}" name="Idea" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{20719C49-147B-4DB6-91D2-A57C1983D59E}" name="Lugar" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{76608A75-85B8-408D-9369-BCFC9E9D7A8A}" name="Nombre" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DE856492-D85D-466F-A960-54F03A0A74D6}" name="Inspiración" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{8733A214-F4B8-45AB-8117-68932FC446F0}" name="Idea" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{20719C49-147B-4DB6-91D2-A57C1983D59E}" name="Lugar" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{C5540FC1-FFBC-4043-8560-7C40AF01B303}" name="Técnica"/>
     <tableColumn id="6" xr3:uid="{028CF8C9-3831-4A85-B60A-3869A589E2E2}" name="Colección"/>
     <tableColumn id="7" xr3:uid="{425AF2BF-72F5-40B1-8952-85F69837C10B}" name="Temática"/>
@@ -4180,22 +4204,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="4" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4659,6 +4684,9 @@
       <c r="H23" t="s">
         <v>110</v>
       </c>
+      <c r="I23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -5468,7 +5496,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44801</v>
       </c>
@@ -5487,7 +5515,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>44808</v>
       </c>
@@ -5509,7 +5537,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>44814</v>
       </c>
@@ -5529,7 +5557,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>44815</v>
       </c>
@@ -5549,7 +5577,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>44821</v>
       </c>
@@ -5569,7 +5597,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>44822</v>
       </c>
@@ -5591,7 +5619,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>44823</v>
       </c>
@@ -5609,8 +5637,11 @@
       <c r="H71" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>44824</v>
       </c>
@@ -5628,8 +5659,11 @@
       <c r="H72" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>44825</v>
       </c>
@@ -5648,7 +5682,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>44826</v>
       </c>
@@ -5668,7 +5702,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>44827</v>
       </c>
@@ -5688,7 +5722,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>44831</v>
       </c>
@@ -5707,7 +5741,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>44833</v>
       </c>
@@ -5726,7 +5760,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>44834</v>
       </c>
@@ -5745,7 +5779,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>44836</v>
       </c>
@@ -5762,7 +5796,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>44840</v>
       </c>
@@ -5780,8 +5814,11 @@
       <c r="H80" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>44843</v>
       </c>
@@ -5803,7 +5840,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>44845</v>
       </c>
@@ -5822,7 +5859,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>44850</v>
       </c>
@@ -5841,7 +5878,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>44855</v>
       </c>
@@ -5861,7 +5898,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>44856</v>
       </c>
@@ -5880,7 +5917,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>44858</v>
       </c>
@@ -5899,7 +5936,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>44864</v>
       </c>
@@ -5921,7 +5958,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>44869</v>
       </c>
@@ -5940,7 +5977,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>44877</v>
       </c>
@@ -5962,7 +5999,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>44878</v>
       </c>
@@ -5984,7 +6021,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>44879</v>
       </c>
@@ -6006,7 +6043,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>44896</v>
       </c>
@@ -6025,7 +6062,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>44903</v>
       </c>
@@ -6043,8 +6080,11 @@
       <c r="H93" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>44912</v>
       </c>
@@ -6063,7 +6103,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>44918</v>
       </c>
@@ -6081,8 +6121,11 @@
       <c r="H95" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>44920</v>
       </c>
@@ -6101,7 +6144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>44922</v>
       </c>
@@ -6123,7 +6166,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>44924</v>
       </c>
@@ -6142,7 +6185,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>44928</v>
       </c>
@@ -6164,7 +6207,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>44930</v>
       </c>
@@ -6181,7 +6224,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>44932</v>
       </c>
@@ -6199,8 +6242,11 @@
       <c r="H101" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I101" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>44937</v>
       </c>
@@ -6218,8 +6264,11 @@
       <c r="H102" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>44939</v>
       </c>
@@ -6236,7 +6285,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>44942</v>
       </c>
@@ -6255,7 +6304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>44943</v>
       </c>
@@ -6274,7 +6323,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>44945</v>
       </c>
@@ -6292,8 +6341,11 @@
       <c r="H106" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>44947</v>
       </c>
@@ -6311,8 +6363,11 @@
       <c r="H107" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I107" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>44955</v>
       </c>
@@ -6331,7 +6386,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>44959</v>
       </c>
@@ -6350,7 +6405,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>44961</v>
       </c>
@@ -6372,7 +6427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>44962</v>
       </c>
@@ -6394,7 +6449,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>44973</v>
       </c>
@@ -6623,9 +6678,31 @@
         <v>110</v>
       </c>
     </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F124" t="s">
+        <v>5</v>
+      </c>
+      <c r="G124" t="s">
+        <v>126</v>
+      </c>
+      <c r="H124" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D113 D115:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
First of the trip
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA63530-783E-4CD6-8530-D9DFBF428E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6D73E-0384-4DFF-B45B-634F26B311EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="185">
   <si>
     <t>Fecha</t>
   </si>
@@ -577,6 +577,24 @@
   </si>
   <si>
     <t>The Somos Bold</t>
+  </si>
+  <si>
+    <t>Philosophers Walk</t>
+  </si>
+  <si>
+    <t>Convocation Hall</t>
+  </si>
+  <si>
+    <t>Niagara Falls</t>
+  </si>
+  <si>
+    <t>Cristina</t>
+  </si>
+  <si>
+    <t>Gloria Vallejo</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -3951,8 +3969,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I131" totalsRowShown="0">
-  <autoFilter ref="A1:I131" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I134" totalsRowShown="0">
+  <autoFilter ref="A1:I134" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4234,10 +4252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4249,7 +4267,8 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" customWidth="1"/>
-    <col min="8" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4387,6 +4406,9 @@
       <c r="H6" t="s">
         <v>111</v>
       </c>
+      <c r="I6" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -6332,6 +6354,9 @@
       <c r="H104" t="s">
         <v>110</v>
       </c>
+      <c r="I104" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
@@ -6351,6 +6376,9 @@
       <c r="H105" t="s">
         <v>110</v>
       </c>
+      <c r="I105" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
@@ -6613,6 +6641,9 @@
       <c r="H118" t="s">
         <v>111</v>
       </c>
+      <c r="I118" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
@@ -6631,6 +6662,9 @@
       </c>
       <c r="H119" t="s">
         <v>110</v>
+      </c>
+      <c r="I119" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -6769,6 +6803,9 @@
       <c r="H126" t="s">
         <v>110</v>
       </c>
+      <c r="I126" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
@@ -6811,7 +6848,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>45046</v>
       </c>
@@ -6833,7 +6870,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>45047</v>
       </c>
@@ -6851,8 +6888,11 @@
       <c r="H130" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>45052</v>
       </c>
@@ -6869,6 +6909,75 @@
       </c>
       <c r="H131" t="s">
         <v>119</v>
+      </c>
+      <c r="I131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>45056</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F132" t="s">
+        <v>5</v>
+      </c>
+      <c r="G132" t="s">
+        <v>173</v>
+      </c>
+      <c r="H132" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C133" s="5"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F133" t="s">
+        <v>5</v>
+      </c>
+      <c r="G133" t="s">
+        <v>173</v>
+      </c>
+      <c r="H133" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>45059</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C134" s="5"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F134" t="s">
+        <v>5</v>
+      </c>
+      <c r="G134" t="s">
+        <v>173</v>
+      </c>
+      <c r="H134" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jpeg to jpg and more paseito
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6D73E-0384-4DFF-B45B-634F26B311EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5C939-78CE-4217-AFC0-656A047E05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="204">
   <si>
     <t>Fecha</t>
   </si>
@@ -561,9 +561,6 @@
     <t>Casa Pedro Nel</t>
   </si>
   <si>
-    <t>Librea Acuarelas 2</t>
-  </si>
-  <si>
     <t>Campos de Paz</t>
   </si>
   <si>
@@ -595,6 +592,66 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>St Joseph</t>
+  </si>
+  <si>
+    <t>Montreal</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 2</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 4</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 5</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 6</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 7</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 8</t>
+  </si>
+  <si>
+    <t>Libreta Acuarelas 9</t>
+  </si>
+  <si>
+    <t>John y Sharon</t>
+  </si>
+  <si>
+    <t>Kathy</t>
+  </si>
+  <si>
+    <t>Charles River</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Isabella Stewart</t>
+  </si>
+  <si>
+    <t>Bear Lake</t>
+  </si>
+  <si>
+    <t>Flatirons</t>
+  </si>
+  <si>
+    <t>Boulder</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>Union Station</t>
+  </si>
+  <si>
+    <t>Denver</t>
   </si>
 </sst>
 </file>
@@ -604,10 +661,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3969,8 +4032,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I134" totalsRowShown="0">
-  <autoFilter ref="A1:I134" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I141" totalsRowShown="0">
+  <autoFilter ref="A1:I141" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4252,10 +4315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4407,7 +4470,7 @@
         <v>111</v>
       </c>
       <c r="I6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -6355,7 +6418,7 @@
         <v>110</v>
       </c>
       <c r="I104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -6377,7 +6440,7 @@
         <v>110</v>
       </c>
       <c r="I105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -6642,7 +6705,7 @@
         <v>111</v>
       </c>
       <c r="I118" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -6664,7 +6727,7 @@
         <v>110</v>
       </c>
       <c r="I119" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -6804,7 +6867,7 @@
         <v>110</v>
       </c>
       <c r="I126" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -6823,7 +6886,7 @@
         <v>5</v>
       </c>
       <c r="G127" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H127" t="s">
         <v>111</v>
@@ -6834,12 +6897,12 @@
         <v>45039</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="7"/>
       <c r="E128" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F128" t="s">
         <v>5</v>
@@ -6853,7 +6916,7 @@
         <v>45046</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C129" s="5"/>
       <c r="D129" s="7"/>
@@ -6864,7 +6927,7 @@
         <v>5</v>
       </c>
       <c r="G129" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H129" t="s">
         <v>110</v>
@@ -6875,7 +6938,7 @@
         <v>45047</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="7"/>
@@ -6889,7 +6952,7 @@
         <v>110</v>
       </c>
       <c r="I130" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -6897,12 +6960,12 @@
         <v>45052</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C131" s="5"/>
       <c r="D131" s="7"/>
       <c r="E131" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F131" t="s">
         <v>5</v>
@@ -6911,7 +6974,7 @@
         <v>119</v>
       </c>
       <c r="I131" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -6919,18 +6982,18 @@
         <v>45056</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="7"/>
       <c r="E132" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F132" t="s">
         <v>5</v>
       </c>
       <c r="G132" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H132" t="s">
         <v>111</v>
@@ -6941,18 +7004,18 @@
         <v>45058</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C133" s="5"/>
       <c r="D133" s="7"/>
       <c r="E133" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F133" t="s">
         <v>5</v>
       </c>
       <c r="G133" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H133" t="s">
         <v>119</v>
@@ -6963,24 +7026,176 @@
         <v>45059</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C134" s="5"/>
       <c r="D134" s="7"/>
       <c r="E134" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F134" t="s">
         <v>5</v>
       </c>
       <c r="G134" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H134" t="s">
         <v>110</v>
       </c>
     </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C135" s="5"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H135" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>45063</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C136" s="5"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F136" t="s">
+        <v>5</v>
+      </c>
+      <c r="G136" t="s">
+        <v>187</v>
+      </c>
+      <c r="H136" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>45065</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C137" s="5"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F137" t="s">
+        <v>5</v>
+      </c>
+      <c r="G137" t="s">
+        <v>188</v>
+      </c>
+      <c r="H137" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>45067</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C138" s="5"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F138" t="s">
+        <v>5</v>
+      </c>
+      <c r="G138" t="s">
+        <v>189</v>
+      </c>
+      <c r="H138" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>45069</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C139" s="5"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F139" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139" t="s">
+        <v>190</v>
+      </c>
+      <c r="H139" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>45072</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F140" t="s">
+        <v>5</v>
+      </c>
+      <c r="G140" t="s">
+        <v>191</v>
+      </c>
+      <c r="H140" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>45079</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C141" s="5"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F141" t="s">
+        <v>5</v>
+      </c>
+      <c r="G141" t="s">
+        <v>192</v>
+      </c>
+      <c r="H141" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:D113 D115:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"x"</formula>

</xml_diff>

<commit_message>
Changes in file structures
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5C939-78CE-4217-AFC0-656A047E05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ABC094-8848-4F71-B9D7-F291F5C42807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="205">
   <si>
     <t>Fecha</t>
   </si>
@@ -603,24 +603,6 @@
     <t>Libreta Acuarelas 2</t>
   </si>
   <si>
-    <t>Libreta Acuarelas 4</t>
-  </si>
-  <si>
-    <t>Libreta Acuarelas 5</t>
-  </si>
-  <si>
-    <t>Libreta Acuarelas 6</t>
-  </si>
-  <si>
-    <t>Libreta Acuarelas 7</t>
-  </si>
-  <si>
-    <t>Libreta Acuarelas 8</t>
-  </si>
-  <si>
-    <t>Libreta Acuarelas 9</t>
-  </si>
-  <si>
     <t>John y Sharon</t>
   </si>
   <si>
@@ -652,6 +634,27 @@
   </si>
   <si>
     <t>Denver</t>
+  </si>
+  <si>
+    <t>Arches National Park</t>
+  </si>
+  <si>
+    <t>Yosemite National Park</t>
+  </si>
+  <si>
+    <t>Grand Canyon National Park</t>
+  </si>
+  <si>
+    <t>Yosemite National Park 2</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Arizona</t>
   </si>
 </sst>
 </file>
@@ -719,6 +722,13 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -734,13 +744,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3759,141 +3762,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="7">
-        <item x="2"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="3"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A15:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
@@ -4031,18 +3900,152 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I141" totalsRowShown="0">
-  <autoFilter ref="A1:I141" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I146" totalsRowShown="0">
+  <autoFilter ref="A1:I146" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{76608A75-85B8-408D-9369-BCFC9E9D7A8A}" name="Nombre" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{DE856492-D85D-466F-A960-54F03A0A74D6}" name="Inspiración" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{8733A214-F4B8-45AB-8117-68932FC446F0}" name="Idea" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{20719C49-147B-4DB6-91D2-A57C1983D59E}" name="Lugar" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{76608A75-85B8-408D-9369-BCFC9E9D7A8A}" name="Nombre" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DE856492-D85D-466F-A960-54F03A0A74D6}" name="Inspiración" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8733A214-F4B8-45AB-8117-68932FC446F0}" name="Idea" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{20719C49-147B-4DB6-91D2-A57C1983D59E}" name="Lugar" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{C5540FC1-FFBC-4043-8560-7C40AF01B303}" name="Técnica"/>
     <tableColumn id="6" xr3:uid="{028CF8C9-3831-4A85-B60A-3869A589E2E2}" name="Colección"/>
     <tableColumn id="7" xr3:uid="{425AF2BF-72F5-40B1-8952-85F69837C10B}" name="Temática"/>
@@ -4315,10 +4318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6727,7 +6730,7 @@
         <v>110</v>
       </c>
       <c r="I119" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -6867,7 +6870,7 @@
         <v>110</v>
       </c>
       <c r="I126" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -7067,18 +7070,18 @@
         <v>45063</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C136" s="5"/>
       <c r="D136" s="7"/>
       <c r="E136" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F136" t="s">
         <v>5</v>
       </c>
       <c r="G136" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H136" t="s">
         <v>111</v>
@@ -7089,18 +7092,18 @@
         <v>45065</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C137" s="5"/>
       <c r="D137" s="7"/>
       <c r="E137" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F137" t="s">
         <v>5</v>
       </c>
       <c r="G137" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H137" t="s">
         <v>111</v>
@@ -7111,18 +7114,18 @@
         <v>45067</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C138" s="5"/>
       <c r="D138" s="7"/>
       <c r="E138" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F138" t="s">
         <v>5</v>
       </c>
       <c r="G138" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H138" t="s">
         <v>110</v>
@@ -7133,18 +7136,18 @@
         <v>45069</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C139" s="5"/>
       <c r="D139" s="7"/>
       <c r="E139" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F139" t="s">
         <v>5</v>
       </c>
       <c r="G139" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H139" t="s">
         <v>110</v>
@@ -7155,18 +7158,18 @@
         <v>45072</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="7"/>
       <c r="E140" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F140" t="s">
         <v>5</v>
       </c>
       <c r="G140" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H140" t="s">
         <v>110</v>
@@ -7177,27 +7180,137 @@
         <v>45079</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C141" s="5"/>
       <c r="D141" s="7"/>
       <c r="E141" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F141" t="s">
         <v>5</v>
       </c>
       <c r="G141" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H141" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>45084</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C142" s="5"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F142" t="s">
+        <v>5</v>
+      </c>
+      <c r="G142" t="s">
+        <v>186</v>
+      </c>
+      <c r="H142" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>45087</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C143" s="5"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F143" t="s">
+        <v>5</v>
+      </c>
+      <c r="G143" t="s">
+        <v>186</v>
+      </c>
+      <c r="H143" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>45099</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C144" s="5"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F144" t="s">
+        <v>5</v>
+      </c>
+      <c r="G144" t="s">
+        <v>186</v>
+      </c>
+      <c r="H144" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>45105</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C145" s="5"/>
+      <c r="D145" s="7"/>
+      <c r="E145" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F145" t="s">
+        <v>5</v>
+      </c>
+      <c r="G145" t="s">
+        <v>186</v>
+      </c>
+      <c r="H145" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>45110</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" s="5"/>
+      <c r="D146" s="7"/>
+      <c r="E146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F146" t="s">
+        <v>5</v>
+      </c>
+      <c r="G146" t="s">
+        <v>186</v>
+      </c>
+      <c r="H146" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:D113 D115:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More art and changes
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ABC094-8848-4F71-B9D7-F291F5C42807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3D670-9E33-4D36-88BA-190992E8E829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="211">
   <si>
     <t>Fecha</t>
   </si>
@@ -655,6 +655,24 @@
   </si>
   <si>
     <t>Arizona</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Matterhorn</t>
+  </si>
+  <si>
+    <t>Volcano</t>
+  </si>
+  <si>
+    <t>Jocelyn Carmes</t>
+  </si>
+  <si>
+    <t>Frederic Church</t>
+  </si>
+  <si>
+    <t>Albert Bierstadt</t>
   </si>
 </sst>
 </file>
@@ -3762,7 +3780,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A15:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
@@ -3901,7 +3919,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
@@ -4035,8 +4053,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I146" totalsRowShown="0">
-  <autoFilter ref="A1:I146" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I149" totalsRowShown="0">
+  <autoFilter ref="A1:I149" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -4318,10 +4336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="I143" sqref="I143"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7305,6 +7323,63 @@
       </c>
       <c r="H146" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>45120</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="1"/>
+      <c r="F147" t="s">
+        <v>5</v>
+      </c>
+      <c r="H147" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>45139</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D148" s="7"/>
+      <c r="E148" s="1"/>
+      <c r="F148" t="s">
+        <v>7</v>
+      </c>
+      <c r="H148" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>45148</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="1"/>
+      <c r="F149" t="s">
+        <v>7</v>
+      </c>
+      <c r="H149" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatic commit of artwork
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3D670-9E33-4D36-88BA-190992E8E829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1180A1-FBD4-4253-B2CA-6FC4D9BF3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="215">
   <si>
     <t>Fecha</t>
   </si>
@@ -673,6 +673,18 @@
   </si>
   <si>
     <t>Albert Bierstadt</t>
+  </si>
+  <si>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>Ángel del Silencio</t>
+  </si>
+  <si>
+    <t>Cementerio San Pedro</t>
+  </si>
+  <si>
+    <t>Casa en llamas</t>
   </si>
 </sst>
 </file>
@@ -3780,6 +3792,140 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A15:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
@@ -3918,145 +4064,11 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="7">
-        <item x="2"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="3"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I149" totalsRowShown="0">
-  <autoFilter ref="A1:I149" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
-    <sortCondition ref="A1:A106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I151" totalsRowShown="0">
+  <autoFilter ref="A1:I151" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I151">
+    <sortCondition descending="1" ref="A1:A151"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="5"/>
@@ -4336,10 +4348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="H150" sqref="H150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4348,7 +4360,7 @@
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="4" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" customWidth="1"/>
     <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
@@ -4386,87 +4398,75 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>44417</v>
+        <v>45170</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>214</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>44418</v>
+        <v>45150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>212</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="7"/>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>44440</v>
+        <v>45148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>44445</v>
+        <v>45139</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="H5" t="s">
         <v>111</v>
@@ -4474,40 +4474,40 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>44446</v>
+        <v>45120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>205</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>111</v>
       </c>
-      <c r="I6" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>44462</v>
+        <v>45110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" t="s">
         <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>186</v>
       </c>
       <c r="H7" t="s">
         <v>111</v>
@@ -4515,303 +4515,342 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>44471</v>
+        <v>45105</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="H8" t="s">
         <v>110</v>
       </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>44487</v>
+        <v>45099</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>200</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
+      <c r="G9" t="s">
+        <v>186</v>
+      </c>
       <c r="H9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>44495</v>
+        <v>45087</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>44507</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>45084</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
+      <c r="G11" t="s">
+        <v>186</v>
+      </c>
       <c r="H11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>44519</v>
+        <v>45079</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>186</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>44526</v>
+        <v>45072</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
+      <c r="G13" t="s">
+        <v>186</v>
+      </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>44532</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>45069</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="C14" s="5"/>
       <c r="D14" s="7"/>
       <c r="E14" s="1" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
+      <c r="G14" t="s">
+        <v>186</v>
+      </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>44558</v>
+        <v>45067</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
+      <c r="G15" t="s">
+        <v>186</v>
+      </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>44564</v>
+        <v>45065</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
+      <c r="G16" t="s">
+        <v>186</v>
+      </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>44567</v>
+        <v>45063</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="7"/>
       <c r="E17" s="1" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>44575</v>
+        <v>45061</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="7"/>
       <c r="E18" s="1" t="s">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>44576</v>
+        <v>45059</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="7"/>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
+      <c r="G19" t="s">
+        <v>186</v>
+      </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>44578</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>45058</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>186</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>44582</v>
+        <v>45056</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
+      <c r="G21" t="s">
+        <v>186</v>
+      </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>44585</v>
+        <v>45052</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F22" t="s">
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="I22" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>44588</v>
+        <v>45047</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="7"/>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="F23" t="s">
         <v>5</v>
@@ -4820,94 +4859,103 @@
         <v>110</v>
       </c>
       <c r="I23" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>44590</v>
+        <v>45046</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="7"/>
       <c r="E24" s="1" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
       </c>
+      <c r="G24" t="s">
+        <v>186</v>
+      </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>44593</v>
+        <v>45039</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
       <c r="E25" s="1" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>44595</v>
+        <v>45038</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>172</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="1" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
       </c>
+      <c r="G26" t="s">
+        <v>186</v>
+      </c>
       <c r="H26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>44597</v>
+        <v>45036</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="I27" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>44600</v>
+        <v>45030</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="1"/>
@@ -4915,61 +4963,66 @@
         <v>5</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="I28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>44604</v>
+        <v>45023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="7"/>
       <c r="E29" s="1" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
       </c>
+      <c r="G29" t="s">
+        <v>126</v>
+      </c>
       <c r="H29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>44614</v>
+        <v>45018</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C30" s="5"/>
       <c r="D30" s="7"/>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
         <v>5</v>
       </c>
       <c r="H30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>44630</v>
+        <v>45017</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="D31" s="7"/>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>126</v>
       </c>
       <c r="H31" t="s">
         <v>111</v>
@@ -4977,16 +5030,14 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>44647</v>
+        <v>45011</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" t="s">
         <v>5</v>
       </c>
@@ -4996,51 +5047,57 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>44650</v>
+        <v>45010</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="7"/>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
         <v>5</v>
       </c>
+      <c r="G33" t="s">
+        <v>126</v>
+      </c>
       <c r="H33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>44653</v>
+        <v>45009</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" t="s">
         <v>5</v>
       </c>
       <c r="H34" t="s">
         <v>110</v>
       </c>
+      <c r="I34" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>44664</v>
-      </c>
-      <c r="B35" s="1"/>
+        <v>45008</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="C35" s="5"/>
       <c r="D35" s="7"/>
       <c r="E35" s="1" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
@@ -5048,156 +5105,163 @@
       <c r="H35" t="s">
         <v>111</v>
       </c>
+      <c r="I35" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>44680</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>45005</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="C36" s="5"/>
       <c r="D36" s="7"/>
       <c r="E36" s="1" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
       </c>
-      <c r="G36" t="s">
-        <v>126</v>
-      </c>
       <c r="H36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>44681</v>
+        <v>45004</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="D37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>44686</v>
+        <v>45001</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E38" s="1"/>
       <c r="F38" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>44689</v>
+        <v>44987</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="7"/>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="I39" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>44693</v>
+        <v>44982</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="F40" t="s">
         <v>5</v>
       </c>
+      <c r="G40" t="s">
+        <v>126</v>
+      </c>
       <c r="H40" t="s">
-        <v>110</v>
-      </c>
-      <c r="I40" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>44697</v>
+        <v>44973</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="E41" s="1"/>
       <c r="F41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>44698</v>
+        <v>44962</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="F42" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>126</v>
       </c>
       <c r="H42" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>44702</v>
-      </c>
-      <c r="B43" s="1"/>
+        <v>44961</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="C43" s="5"/>
       <c r="D43" s="7"/>
       <c r="E43" s="1" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="F43" t="s">
         <v>5</v>
@@ -5206,43 +5270,42 @@
         <v>126</v>
       </c>
       <c r="H43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>44703</v>
+        <v>44959</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E44" s="1"/>
       <c r="F44" t="s">
         <v>5</v>
       </c>
       <c r="H44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>44705</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>44955</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C45" s="5"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="D45" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="1"/>
       <c r="F45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="H45" t="s">
         <v>110</v>
@@ -5250,179 +5313,181 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>44709</v>
+        <v>44947</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="7"/>
       <c r="E46" s="1" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="F46" t="s">
         <v>5</v>
-      </c>
-      <c r="G46" t="s">
-        <v>126</v>
       </c>
       <c r="H46" t="s">
         <v>111</v>
       </c>
+      <c r="I46" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>44713</v>
+        <v>44945</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="I47" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>44727</v>
+        <v>44943</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>44728</v>
+        <v>44942</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E49" s="1"/>
       <c r="F49" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="H49" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>44731</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="1"/>
+        <v>44939</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F50" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>126</v>
       </c>
       <c r="H50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>44734</v>
+        <v>44937</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="D51" s="7"/>
       <c r="E51" s="1"/>
       <c r="F51" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H51" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>44738</v>
+        <v>44932</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="D52" s="7"/>
-      <c r="E52" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" t="s">
-        <v>5</v>
-      </c>
-      <c r="G52" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="H52" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <v>44740</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53" s="5"/>
+        <v>44930</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D53" s="7"/>
-      <c r="E53" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="E53" s="1"/>
       <c r="F53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>44745</v>
-      </c>
-      <c r="B54" s="1"/>
+        <v>44928</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C54" s="5"/>
       <c r="D54" s="7"/>
       <c r="E54" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F54" t="s">
         <v>5</v>
@@ -5434,37 +5499,36 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>44746</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="5"/>
+        <v>44924</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="D55" s="7"/>
-      <c r="E55" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" t="s">
-        <v>5</v>
-      </c>
-      <c r="G55" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>44747</v>
+        <v>44922</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="7"/>
       <c r="E56" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F56" t="s">
         <v>5</v>
@@ -5473,120 +5537,122 @@
         <v>126</v>
       </c>
       <c r="H56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>44920</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>44753</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F57" t="s">
-        <v>5</v>
-      </c>
-      <c r="G57" t="s">
-        <v>126</v>
-      </c>
-      <c r="H57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>44758</v>
-      </c>
-      <c r="B58" s="1"/>
+        <v>44918</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C58" s="5"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="D58" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="1"/>
       <c r="F58" t="s">
         <v>5</v>
       </c>
-      <c r="G58" t="s">
-        <v>126</v>
-      </c>
       <c r="H58" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="I58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <v>44760</v>
-      </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="5"/>
+        <v>44912</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D59" s="7"/>
-      <c r="E59" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E59" s="1"/>
       <c r="F59" t="s">
         <v>5</v>
       </c>
-      <c r="G59" t="s">
-        <v>126</v>
-      </c>
       <c r="H59" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>44770</v>
+        <v>44903</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="D60" s="7"/>
-      <c r="E60" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E60" s="1"/>
       <c r="F60" t="s">
-        <v>8</v>
-      </c>
-      <c r="G60" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="I60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <v>44782</v>
+        <v>44896</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="7"/>
       <c r="E61" s="1"/>
       <c r="F61" t="s">
         <v>5</v>
       </c>
       <c r="H61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>44784</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>44879</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" s="5"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F62" t="s">
         <v>5</v>
       </c>
@@ -5594,32 +5660,42 @@
         <v>126</v>
       </c>
       <c r="H62" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <v>44790</v>
-      </c>
-      <c r="B63" s="1"/>
+        <v>44878</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C63" s="5"/>
       <c r="D63" s="7"/>
       <c r="E63" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F63" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>126</v>
       </c>
       <c r="H63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>44793</v>
-      </c>
+        <v>44877</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="7"/>
       <c r="E64" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F64" t="s">
         <v>5</v>
@@ -5628,40 +5704,40 @@
         <v>126</v>
       </c>
       <c r="H64" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>44801</v>
+        <v>44869</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C65" s="5"/>
-      <c r="D65" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E65" s="1"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F65" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H65" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>44808</v>
+        <v>44864</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C66" s="5"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F66" t="s">
         <v>5</v>
       </c>
@@ -5674,53 +5750,51 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>44814</v>
-      </c>
-      <c r="B67" s="1"/>
+        <v>44858</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="D67" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="1"/>
       <c r="F67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G67" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H67" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>44815</v>
-      </c>
-      <c r="B68" s="1"/>
+        <v>44856</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C68" s="5"/>
       <c r="D68" s="7"/>
       <c r="E68" s="1" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="F68" t="s">
         <v>5</v>
       </c>
-      <c r="G68" t="s">
-        <v>126</v>
-      </c>
       <c r="H68" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <v>44821</v>
+        <v>44855</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="5"/>
       <c r="D69" s="7"/>
       <c r="E69" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F69" t="s">
         <v>5</v>
@@ -5734,76 +5808,70 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <v>44822</v>
+        <v>44850</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="7"/>
       <c r="E70" s="1"/>
       <c r="F70" t="s">
         <v>8</v>
       </c>
-      <c r="G70" t="s">
-        <v>121</v>
-      </c>
       <c r="H70" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <v>44823</v>
+        <v>44845</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>37</v>
+        <v>147</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="1"/>
       <c r="F71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>110</v>
-      </c>
-      <c r="I71" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>44824</v>
+        <v>44843</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C72" s="5"/>
       <c r="D72" s="7"/>
-      <c r="E72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F72" t="s">
         <v>5</v>
       </c>
+      <c r="G72" t="s">
+        <v>126</v>
+      </c>
       <c r="H72" t="s">
-        <v>110</v>
-      </c>
-      <c r="I72" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
-        <v>44825</v>
+        <v>44840</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>37</v>
@@ -5811,58 +5879,57 @@
       <c r="D73" s="7"/>
       <c r="E73" s="1"/>
       <c r="F73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H73" t="s">
         <v>111</v>
       </c>
+      <c r="I73" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
-        <v>44826</v>
+        <v>44836</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="5"/>
       <c r="D74" s="7"/>
       <c r="E74" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F74" t="s">
         <v>5</v>
       </c>
-      <c r="G74" t="s">
-        <v>126</v>
-      </c>
       <c r="H74" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
-        <v>44827</v>
-      </c>
-      <c r="B75" s="1"/>
+        <v>44834</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C75" s="5"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D75" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="1"/>
       <c r="F75" t="s">
-        <v>5</v>
-      </c>
-      <c r="G75" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="H75" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
-        <v>44831</v>
+        <v>44833</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="7" t="s">
@@ -5873,15 +5940,15 @@
         <v>6</v>
       </c>
       <c r="H76" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
-        <v>44833</v>
+        <v>44831</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="7" t="s">
@@ -5892,51 +5959,55 @@
         <v>6</v>
       </c>
       <c r="H77" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
-        <v>44834</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>44827</v>
+      </c>
+      <c r="B78" s="1"/>
       <c r="C78" s="5"/>
-      <c r="D78" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E78" s="1"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F78" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="G78" t="s">
+        <v>126</v>
       </c>
       <c r="H78" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
-        <v>44836</v>
+        <v>44826</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="5"/>
       <c r="D79" s="7"/>
       <c r="E79" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F79" t="s">
         <v>5</v>
       </c>
+      <c r="G79" t="s">
+        <v>126</v>
+      </c>
       <c r="H79" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
-        <v>44840</v>
+        <v>44825</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>37</v>
@@ -5944,84 +6015,87 @@
       <c r="D80" s="7"/>
       <c r="E80" s="1"/>
       <c r="F80" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H80" t="s">
         <v>111</v>
       </c>
-      <c r="I80" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
-        <v>44843</v>
+        <v>44824</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C81" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D81" s="7"/>
-      <c r="E81" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E81" s="1"/>
       <c r="F81" t="s">
         <v>5</v>
       </c>
-      <c r="G81" t="s">
-        <v>126</v>
-      </c>
       <c r="H81" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="I81" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
-        <v>44845</v>
+        <v>44823</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="1"/>
       <c r="F82" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H82" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="I82" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
-        <v>44850</v>
+        <v>44822</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D83" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E83" s="1"/>
       <c r="F83" t="s">
         <v>8</v>
       </c>
+      <c r="G83" t="s">
+        <v>121</v>
+      </c>
       <c r="H83" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>44855</v>
+        <v>44821</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="5"/>
       <c r="D84" s="7"/>
       <c r="E84" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F84" t="s">
         <v>5</v>
@@ -6035,54 +6109,56 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
-        <v>44856</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>44815</v>
+      </c>
+      <c r="B85" s="1"/>
       <c r="C85" s="5"/>
       <c r="D85" s="7"/>
       <c r="E85" s="1" t="s">
-        <v>133</v>
+        <v>40</v>
       </c>
       <c r="F85" t="s">
         <v>5</v>
       </c>
+      <c r="G85" t="s">
+        <v>126</v>
+      </c>
       <c r="H85" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
-        <v>44858</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>44814</v>
+      </c>
+      <c r="B86" s="1"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E86" s="1"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F86" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G86" t="s">
+        <v>126</v>
       </c>
       <c r="H86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
-        <v>44864</v>
+        <v>44808</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D87" s="7"/>
-      <c r="E87" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E87" s="1"/>
       <c r="F87" t="s">
         <v>5</v>
       </c>
@@ -6095,34 +6171,29 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
-        <v>44869</v>
+        <v>44801</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C88" s="5"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D88" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E88" s="1"/>
       <c r="F88" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H88" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
-        <v>44877</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="7"/>
+        <v>44793</v>
+      </c>
       <c r="E89" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F89" t="s">
         <v>5</v>
@@ -6131,26 +6202,21 @@
         <v>126</v>
       </c>
       <c r="H89" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
-        <v>44878</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>99</v>
-      </c>
+        <v>44790</v>
+      </c>
+      <c r="B90" s="1"/>
       <c r="C90" s="5"/>
       <c r="D90" s="7"/>
       <c r="E90" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H90" t="s">
         <v>110</v>
@@ -6158,16 +6224,14 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
-        <v>44879</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C91" s="5"/>
+        <v>44784</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D91" s="7"/>
-      <c r="E91" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E91" s="1"/>
       <c r="F91" t="s">
         <v>5</v>
       </c>
@@ -6175,121 +6239,121 @@
         <v>126</v>
       </c>
       <c r="H91" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
-        <v>44896</v>
+        <v>44782</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="D92" s="7"/>
       <c r="E92" s="1"/>
       <c r="F92" t="s">
         <v>5</v>
       </c>
       <c r="H92" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
-        <v>44903</v>
+        <v>44770</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C93" s="5"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="1"/>
+      <c r="E93" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F93" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="G93" t="s">
+        <v>121</v>
       </c>
       <c r="H93" t="s">
-        <v>114</v>
-      </c>
-      <c r="I93" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
-        <v>44912</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>44760</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="5"/>
       <c r="D94" s="7"/>
-      <c r="E94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F94" t="s">
         <v>5</v>
       </c>
+      <c r="G94" t="s">
+        <v>126</v>
+      </c>
       <c r="H94" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
-        <v>44918</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>44758</v>
+      </c>
+      <c r="B95" s="1"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E95" s="1"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F95" t="s">
         <v>5</v>
       </c>
+      <c r="G95" t="s">
+        <v>126</v>
+      </c>
       <c r="H95" t="s">
-        <v>114</v>
-      </c>
-      <c r="I95" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
-        <v>44920</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>44753</v>
+      </c>
+      <c r="B96" s="1"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E96" s="1"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F96" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="G96" t="s">
+        <v>126</v>
       </c>
       <c r="H96" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
-        <v>44922</v>
+        <v>44747</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="7"/>
       <c r="E97" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="F97" t="s">
         <v>5</v>
@@ -6298,39 +6362,38 @@
         <v>126</v>
       </c>
       <c r="H97" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>44746</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" t="s">
+        <v>126</v>
+      </c>
+      <c r="H98" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="2">
-        <v>44924</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D98" s="7"/>
-      <c r="E98" s="1"/>
-      <c r="F98" t="s">
-        <v>6</v>
-      </c>
-      <c r="H98" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
-        <v>44928</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>44745</v>
+      </c>
+      <c r="B99" s="1"/>
       <c r="C99" s="5"/>
       <c r="D99" s="7"/>
       <c r="E99" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="F99" t="s">
         <v>5</v>
@@ -6342,221 +6405,220 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
-        <v>44930</v>
-      </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>44740</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C100" s="5"/>
       <c r="D100" s="7"/>
-      <c r="E100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="F100" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H100" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
-        <v>44932</v>
+        <v>44738</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>146</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C101" s="5"/>
       <c r="D101" s="7"/>
-      <c r="E101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F101" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G101" t="s">
+        <v>126</v>
       </c>
       <c r="H101" t="s">
         <v>111</v>
       </c>
-      <c r="I101" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
-        <v>44937</v>
+        <v>44734</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C102" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C102" s="5"/>
+      <c r="D102" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D102" s="7"/>
       <c r="E102" s="1"/>
       <c r="F102" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H102" t="s">
         <v>111</v>
       </c>
-      <c r="I102" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
-        <v>44939</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>44731</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="1"/>
       <c r="F103" t="s">
-        <v>5</v>
-      </c>
-      <c r="G103" t="s">
+        <v>8</v>
+      </c>
+      <c r="H103" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>44728</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F104" t="s">
+        <v>5</v>
+      </c>
+      <c r="G104" t="s">
         <v>126</v>
-      </c>
-      <c r="H103" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>44942</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D104" s="7"/>
-      <c r="E104" s="1"/>
-      <c r="F104" t="s">
-        <v>4</v>
       </c>
       <c r="H104" t="s">
         <v>110</v>
       </c>
-      <c r="I104" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
-        <v>44943</v>
+        <v>44727</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C105" s="5"/>
       <c r="D105" s="7"/>
-      <c r="E105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F105" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G105" t="s">
+        <v>126</v>
       </c>
       <c r="H105" t="s">
-        <v>110</v>
-      </c>
-      <c r="I105" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
-        <v>44945</v>
+        <v>44713</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C106" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D106" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H106" t="s">
-        <v>110</v>
-      </c>
-      <c r="I106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
-        <v>44947</v>
+        <v>44709</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="7"/>
       <c r="E107" s="1" t="s">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="F107" t="s">
         <v>5</v>
+      </c>
+      <c r="G107" t="s">
+        <v>126</v>
       </c>
       <c r="H107" t="s">
         <v>111</v>
       </c>
-      <c r="I107" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
-        <v>44955</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>136</v>
-      </c>
+        <v>44705</v>
+      </c>
+      <c r="B108" s="1"/>
       <c r="C108" s="5"/>
-      <c r="D108" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E108" s="1"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F108" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="G108" t="s">
+        <v>126</v>
       </c>
       <c r="H108" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
-        <v>44959</v>
+        <v>44703</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D109" s="7"/>
       <c r="E109" s="1"/>
       <c r="F109" t="s">
         <v>5</v>
       </c>
       <c r="H109" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
-        <v>44961</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>44702</v>
+      </c>
+      <c r="B110" s="1"/>
       <c r="C110" s="5"/>
       <c r="D110" s="7"/>
       <c r="E110" s="1" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="F110" t="s">
         <v>5</v>
@@ -6565,159 +6627,158 @@
         <v>126</v>
       </c>
       <c r="H110" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
-        <v>44962</v>
+        <v>44698</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C111" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D111" s="7"/>
-      <c r="E111" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="E111" s="1"/>
       <c r="F111" t="s">
-        <v>5</v>
-      </c>
-      <c r="G111" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
-        <v>44973</v>
+        <v>44697</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>145</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C112" s="5"/>
       <c r="D112" s="7"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F112" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H112" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
-        <v>44982</v>
+        <v>44693</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C113" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="D113" s="7"/>
-      <c r="E113" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="E113" s="1"/>
       <c r="F113" t="s">
         <v>5</v>
       </c>
-      <c r="G113" t="s">
-        <v>126</v>
-      </c>
       <c r="H113" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="I113" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
-        <v>44987</v>
+        <v>44689</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D114" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E114" s="1"/>
       <c r="F114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H114" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
-        <v>45001</v>
+        <v>44686</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>144</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C115" s="5"/>
       <c r="D115" s="7"/>
-      <c r="E115" s="1"/>
+      <c r="E115" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F115" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H115" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
-        <v>45004</v>
+        <v>44681</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="C116" s="5"/>
-      <c r="D116" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E116" s="1"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F116" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G116" t="s">
+        <v>126</v>
       </c>
       <c r="H116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
-        <v>45005</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>151</v>
-      </c>
+        <v>44680</v>
+      </c>
+      <c r="B117" s="1"/>
       <c r="C117" s="5"/>
       <c r="D117" s="7"/>
       <c r="E117" s="1" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="F117" t="s">
         <v>5</v>
       </c>
+      <c r="G117" t="s">
+        <v>126</v>
+      </c>
       <c r="H117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
-        <v>45008</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>44664</v>
+      </c>
+      <c r="B118" s="1"/>
       <c r="C118" s="5"/>
       <c r="D118" s="7"/>
       <c r="E118" s="1" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="F118" t="s">
         <v>5</v>
@@ -6725,62 +6786,57 @@
       <c r="H118" t="s">
         <v>111</v>
       </c>
-      <c r="I118" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
-        <v>45009</v>
+        <v>44653</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C119" s="5"/>
       <c r="D119" s="7"/>
-      <c r="E119" s="1"/>
+      <c r="E119" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F119" t="s">
         <v>5</v>
       </c>
       <c r="H119" t="s">
         <v>110</v>
       </c>
-      <c r="I119" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
-        <v>45010</v>
+        <v>44650</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C120" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D120" s="7"/>
       <c r="E120" s="1"/>
       <c r="F120" t="s">
         <v>5</v>
       </c>
-      <c r="G120" t="s">
-        <v>126</v>
-      </c>
       <c r="H120" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
-        <v>45011</v>
+        <v>44647</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="C121" s="5"/>
       <c r="D121" s="7"/>
-      <c r="E121" s="1"/>
+      <c r="E121" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F121" t="s">
         <v>5</v>
       </c>
@@ -6790,19 +6846,18 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
-        <v>45017</v>
+        <v>44630</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="C122" s="5"/>
-      <c r="D122" s="7"/>
+      <c r="D122" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E122" s="1"/>
       <c r="F122" t="s">
-        <v>5</v>
-      </c>
-      <c r="G122" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H122" t="s">
         <v>111</v>
@@ -6810,52 +6865,51 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>45018</v>
+        <v>44614</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C123" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D123" s="7"/>
       <c r="E123" s="1"/>
       <c r="F123" t="s">
         <v>5</v>
       </c>
       <c r="H123" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>45023</v>
+        <v>44604</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="7"/>
       <c r="E124" s="1" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="F124" t="s">
         <v>5</v>
       </c>
-      <c r="G124" t="s">
-        <v>126</v>
-      </c>
       <c r="H124" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>45030</v>
+        <v>44600</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>169</v>
+        <v>77</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="1"/>
@@ -6863,108 +6917,96 @@
         <v>5</v>
       </c>
       <c r="H125" t="s">
-        <v>110</v>
-      </c>
-      <c r="I125" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>45036</v>
+        <v>44597</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C126" s="5"/>
       <c r="D126" s="7"/>
-      <c r="E126" s="1"/>
+      <c r="E126" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F126" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H126" t="s">
-        <v>110</v>
-      </c>
-      <c r="I126" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>45038</v>
+        <v>44595</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="C127" s="5"/>
       <c r="D127" s="7"/>
       <c r="E127" s="1" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="F127" t="s">
         <v>5</v>
       </c>
-      <c r="G127" t="s">
-        <v>186</v>
-      </c>
       <c r="H127" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>45039</v>
+        <v>44593</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>173</v>
+        <v>26</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="7"/>
       <c r="E128" s="1" t="s">
-        <v>173</v>
+        <v>26</v>
       </c>
       <c r="F128" t="s">
         <v>5</v>
       </c>
       <c r="H128" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>45046</v>
+        <v>44590</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="C129" s="5"/>
       <c r="D129" s="7"/>
       <c r="E129" s="1" t="s">
-        <v>154</v>
+        <v>41</v>
       </c>
       <c r="F129" t="s">
         <v>5</v>
       </c>
-      <c r="G129" t="s">
-        <v>186</v>
-      </c>
       <c r="H129" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
-        <v>45047</v>
+        <v>44588</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>175</v>
+        <v>80</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="7"/>
       <c r="E130" s="1" t="s">
-        <v>154</v>
+        <v>19</v>
       </c>
       <c r="F130" t="s">
         <v>5</v>
@@ -6973,418 +7015,429 @@
         <v>110</v>
       </c>
       <c r="I130" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
-        <v>45052</v>
+        <v>44585</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C131" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D131" s="7"/>
-      <c r="E131" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="E131" s="1"/>
       <c r="F131" t="s">
         <v>5</v>
       </c>
       <c r="H131" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I131" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
-        <v>45056</v>
+        <v>44582</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C132" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D132" s="7"/>
-      <c r="E132" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="E132" s="1"/>
       <c r="F132" t="s">
         <v>5</v>
       </c>
-      <c r="G132" t="s">
-        <v>186</v>
-      </c>
       <c r="H132" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
-        <v>45058</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>179</v>
-      </c>
+        <v>44578</v>
+      </c>
+      <c r="B133" s="1"/>
       <c r="C133" s="5"/>
       <c r="D133" s="7"/>
       <c r="E133" s="1" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="F133" t="s">
-        <v>5</v>
-      </c>
-      <c r="G133" t="s">
-        <v>186</v>
+        <v>6</v>
       </c>
       <c r="H133" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
-        <v>45059</v>
+        <v>44576</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C134" s="5"/>
       <c r="D134" s="7"/>
       <c r="E134" s="1" t="s">
-        <v>180</v>
+        <v>56</v>
       </c>
       <c r="F134" t="s">
         <v>5</v>
       </c>
-      <c r="G134" t="s">
-        <v>186</v>
-      </c>
       <c r="H134" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
-        <v>45061</v>
+        <v>44575</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>184</v>
+        <v>84</v>
       </c>
       <c r="C135" s="5"/>
       <c r="D135" s="7"/>
       <c r="E135" s="1" t="s">
-        <v>185</v>
+        <v>85</v>
       </c>
       <c r="F135" t="s">
         <v>5</v>
       </c>
       <c r="H135" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
-        <v>45063</v>
+        <v>44567</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
       <c r="C136" s="5"/>
       <c r="D136" s="7"/>
       <c r="E136" s="1" t="s">
-        <v>190</v>
+        <v>85</v>
       </c>
       <c r="F136" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G136" t="s">
-        <v>186</v>
+        <v>121</v>
       </c>
       <c r="H136" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
-        <v>45065</v>
+        <v>44564</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C137" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D137" s="7"/>
-      <c r="E137" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="E137" s="1"/>
       <c r="F137" t="s">
         <v>5</v>
       </c>
-      <c r="G137" t="s">
-        <v>186</v>
-      </c>
       <c r="H137" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
-        <v>45067</v>
+        <v>44558</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C138" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D138" s="7"/>
-      <c r="E138" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="E138" s="1"/>
       <c r="F138" t="s">
         <v>5</v>
       </c>
-      <c r="G138" t="s">
-        <v>186</v>
-      </c>
       <c r="H138" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
-        <v>45069</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>193</v>
-      </c>
+        <v>44532</v>
+      </c>
+      <c r="B139" s="1"/>
       <c r="C139" s="5"/>
       <c r="D139" s="7"/>
       <c r="E139" s="1" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="F139" t="s">
         <v>5</v>
       </c>
-      <c r="G139" t="s">
-        <v>186</v>
-      </c>
       <c r="H139" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
-        <v>45072</v>
+        <v>44526</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C140" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D140" s="7"/>
-      <c r="E140" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="E140" s="1"/>
       <c r="F140" t="s">
         <v>5</v>
       </c>
-      <c r="G140" t="s">
-        <v>186</v>
-      </c>
       <c r="H140" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
-        <v>45079</v>
+        <v>44519</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>196</v>
+        <v>90</v>
       </c>
       <c r="C141" s="5"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="D141" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E141" s="1"/>
       <c r="F141" t="s">
-        <v>5</v>
-      </c>
-      <c r="G141" t="s">
-        <v>186</v>
+        <v>6</v>
       </c>
       <c r="H141" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
-        <v>45084</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>198</v>
-      </c>
+        <v>44507</v>
+      </c>
+      <c r="B142" s="1"/>
       <c r="C142" s="5"/>
       <c r="D142" s="7"/>
       <c r="E142" s="1" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="F142" t="s">
         <v>5</v>
       </c>
-      <c r="G142" t="s">
-        <v>186</v>
-      </c>
       <c r="H142" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
-        <v>45087</v>
+        <v>44495</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C143" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D143" s="7"/>
-      <c r="E143" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="E143" s="1"/>
       <c r="F143" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G143" t="s">
-        <v>186</v>
+        <v>121</v>
       </c>
       <c r="H143" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
-        <v>45099</v>
+        <v>44487</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>200</v>
+        <v>19</v>
       </c>
       <c r="C144" s="5"/>
       <c r="D144" s="7"/>
       <c r="E144" s="1" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="F144" t="s">
         <v>5</v>
       </c>
-      <c r="G144" t="s">
-        <v>186</v>
-      </c>
       <c r="H144" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
-        <v>45105</v>
+        <v>44471</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C145" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D145" s="7"/>
-      <c r="E145" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="E145" s="1"/>
       <c r="F145" t="s">
         <v>5</v>
-      </c>
-      <c r="G145" t="s">
-        <v>186</v>
       </c>
       <c r="H145" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
-        <v>45110</v>
+        <v>44462</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C146" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D146" s="7"/>
-      <c r="E146" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E146" s="1"/>
       <c r="F146" t="s">
         <v>5</v>
-      </c>
-      <c r="G146" t="s">
-        <v>186</v>
       </c>
       <c r="H146" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
-        <v>45120</v>
+        <v>44446</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>209</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C147" s="5"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="1"/>
+      <c r="E147" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F147" t="s">
         <v>5</v>
       </c>
       <c r="H147" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I147" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
-        <v>45139</v>
+        <v>44445</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>207</v>
+        <v>95</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="D148" s="7"/>
       <c r="E148" s="1"/>
       <c r="F148" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="G148" t="s">
+        <v>121</v>
       </c>
       <c r="H148" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
-        <v>45148</v>
+        <v>44440</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>210</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C149" s="5"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="1"/>
+      <c r="E149" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F149" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="G149" t="s">
+        <v>121</v>
       </c>
       <c r="H149" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>44418</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C150" s="5"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F150" t="s">
+        <v>9</v>
+      </c>
+      <c r="G150" t="s">
+        <v>121</v>
+      </c>
+      <c r="H150" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>44417</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C151" s="5"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F151" t="s">
+        <v>9</v>
+      </c>
+      <c r="G151" t="s">
+        <v>121</v>
+      </c>
+      <c r="H151" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D113 D115:D1048576">
+  <conditionalFormatting sqref="D1:D115 D117:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Arte y modo darks
</commit_message>
<xml_diff>
--- a/assets/art/art.xlsx
+++ b/assets/art/art.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgustinVallejo\Documents\AgustinVallejo.github.io\assets\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CA6304-FB91-4F50-BF10-1B08334BA952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF2E041-F412-4100-8CE2-2E12F26881E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="254">
   <si>
     <t>Fecha</t>
   </si>
@@ -799,6 +799,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>C4TA</t>
   </si>
 </sst>
 </file>
@@ -3906,6 +3909,140 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16ABB999-28BC-4290-8192-E4E791ADED20}" name="TablaDinámica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A15:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
@@ -4044,145 +4181,11 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{619BF6E1-974F-49C1-A212-5849F36FBC3D}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="7">
-        <item x="2"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="3"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de Temática" fld="6" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I172" totalsRowShown="0">
-  <autoFilter ref="A1:I172" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I172">
-    <sortCondition descending="1" ref="A1:A172"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}" name="Tabla1" displayName="Tabla1" ref="A1:I173" totalsRowShown="0">
+  <autoFilter ref="A1:I173" xr:uid="{FB7C0B72-DEDB-4330-B45F-99A88E97EBC0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I173">
+    <sortCondition descending="1" ref="A1:A173"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0B5B84D9-04FF-4EA5-A456-93D6EAF0117B}" name="Fecha" dataDxfId="5"/>
@@ -4462,10 +4465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I172"/>
+  <dimension ref="A1:I173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4512,59 +4515,62 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>45419</v>
+        <v>45423</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" t="s">
+        <v>186</v>
+      </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45394</v>
+        <v>45419</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="1" t="s">
-        <v>250</v>
-      </c>
+      <c r="D3" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>186</v>
-      </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>45339</v>
+        <v>45394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7"/>
       <c r="E4" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>186</v>
       </c>
       <c r="H4" t="s">
         <v>119</v>
@@ -4572,56 +4578,53 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>45330</v>
+        <v>45339</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>208</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="F5" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>45318</v>
+        <v>45330</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>243</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="H6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>45314</v>
+        <v>45318</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="7"/>
       <c r="E7" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -4630,15 +4633,15 @@
         <v>186</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>45313</v>
+        <v>45314</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="7"/>
@@ -4657,15 +4660,15 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>45312</v>
+        <v>45313</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -4679,37 +4682,40 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>45307</v>
+        <v>45312</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="7"/>
       <c r="E10" s="1" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
+      <c r="G10" t="s">
+        <v>186</v>
+      </c>
       <c r="H10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>45295</v>
+        <v>45307</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>237</v>
+        <v>132</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
@@ -4719,235 +4725,235 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>45286</v>
+        <v>45295</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" s="5"/>
+        <v>236</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" t="s">
-        <v>186</v>
-      </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>45265</v>
+        <v>45286</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
+      <c r="G13" t="s">
+        <v>186</v>
+      </c>
       <c r="H13" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>45264</v>
+        <v>45265</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="7"/>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
-      </c>
-      <c r="I14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>45244</v>
+        <v>45264</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>229</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="7"/>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
         <v>220</v>
       </c>
       <c r="H15" t="s">
-        <v>230</v>
+        <v>114</v>
+      </c>
+      <c r="I15" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>45234</v>
+        <v>45244</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>228</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45225</v>
+        <v>45234</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>225</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="F17" t="s">
-        <v>220</v>
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>186</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45213</v>
+        <v>45225</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>223</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>45193</v>
+        <v>45213</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="7"/>
       <c r="E19" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
+      <c r="G19" t="s">
+        <v>186</v>
+      </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>45188</v>
+        <v>45193</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>219</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="F20" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>45179</v>
+        <v>45188</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>45178</v>
+        <v>45179</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>217</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" t="s">
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>45170</v>
+        <v>45178</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>208</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="F23" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H23" t="s">
         <v>111</v>
@@ -4955,51 +4961,51 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>45150</v>
+        <v>45170</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>214</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>45148</v>
+        <v>45150</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>210</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="F25" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>45139</v>
+        <v>45148</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="1"/>
@@ -5007,23 +5013,23 @@
         <v>220</v>
       </c>
       <c r="H26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>45120</v>
+        <v>45139</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H27" t="s">
         <v>111</v>
@@ -5031,21 +5037,18 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>45110</v>
+        <v>45120</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="5"/>
+        <v>205</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" t="s">
         <v>5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>186</v>
       </c>
       <c r="H28" t="s">
         <v>111</v>
@@ -5053,59 +5056,59 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>45105</v>
+        <v>45110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>201</v>
+        <v>19</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="7"/>
       <c r="E29" s="1" t="s">
-        <v>203</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
       </c>
+      <c r="G29" t="s">
+        <v>186</v>
+      </c>
       <c r="H29" t="s">
-        <v>110</v>
-      </c>
-      <c r="I29" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>45099</v>
+        <v>45105</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="7"/>
       <c r="E30" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F30" t="s">
         <v>5</v>
-      </c>
-      <c r="G30" t="s">
-        <v>186</v>
       </c>
       <c r="H30" t="s">
         <v>110</v>
       </c>
+      <c r="I30" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>45087</v>
+        <v>45099</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
       <c r="E31" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -5119,15 +5122,15 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>45084</v>
+        <v>45087</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
       <c r="E32" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
@@ -5141,15 +5144,15 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>45079</v>
+        <v>45084</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="7"/>
       <c r="E33" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F33" t="s">
         <v>5</v>
@@ -5158,20 +5161,20 @@
         <v>186</v>
       </c>
       <c r="H33" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>45072</v>
+        <v>45079</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="7"/>
       <c r="E34" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F34" t="s">
         <v>5</v>
@@ -5180,15 +5183,15 @@
         <v>186</v>
       </c>
       <c r="H34" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>45069</v>
+        <v>45072</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="7"/>
@@ -5207,10 +5210,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>45067</v>
+        <v>45069</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="7"/>
@@ -5229,15 +5232,15 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>45065</v>
+        <v>45067</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="7"/>
       <c r="E37" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
@@ -5246,15 +5249,15 @@
         <v>186</v>
       </c>
       <c r="H37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="7"/>
@@ -5273,56 +5276,56 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>45061</v>
+        <v>45063</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="7"/>
       <c r="E39" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F39" t="s">
         <v>5</v>
       </c>
+      <c r="G39" t="s">
+        <v>186</v>
+      </c>
       <c r="H39" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>45059</v>
+        <v>45061</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="7"/>
       <c r="E40" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
       </c>
-      <c r="G40" t="s">
-        <v>186</v>
-      </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>45058</v>
+        <v>45059</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="7"/>
       <c r="E41" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F41" t="s">
         <v>5</v>
@@ -5331,20 +5334,20 @@
         <v>186</v>
       </c>
       <c r="H41" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>45056</v>
+        <v>45058</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="7"/>
       <c r="E42" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
@@ -5353,56 +5356,59 @@
         <v>186</v>
       </c>
       <c r="H42" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>45052</v>
+        <v>45056</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="7"/>
       <c r="E43" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F43" t="s">
         <v>5</v>
       </c>
+      <c r="G43" t="s">
+        <v>186</v>
+      </c>
       <c r="H43" t="s">
-        <v>119</v>
-      </c>
-      <c r="I43" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>45047</v>
+        <v>45052</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="7"/>
       <c r="E44" s="1" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
       </c>
       <c r="H44" t="s">
-        <v>110</v>
+        <v>119</v>
+      </c>
+      <c r="I44" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>45046</v>
+        <v>45047</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="7"/>
@@ -5412,132 +5418,134 @@
       <c r="F45" t="s">
         <v>5</v>
       </c>
-      <c r="G45" t="s">
-        <v>186</v>
-      </c>
       <c r="H45" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>45039</v>
+        <v>45046</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="7"/>
       <c r="E46" s="1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F46" t="s">
         <v>5</v>
       </c>
+      <c r="G46" t="s">
+        <v>186</v>
+      </c>
       <c r="H46" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>45038</v>
+        <v>45039</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="7"/>
       <c r="E47" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F47" t="s">
         <v>5</v>
       </c>
-      <c r="G47" t="s">
-        <v>186</v>
-      </c>
       <c r="H47" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>45036</v>
+        <v>45038</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C48" s="5"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="F48" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>186</v>
       </c>
       <c r="H48" t="s">
-        <v>110</v>
-      </c>
-      <c r="I48" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>45030</v>
+        <v>45036</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="1"/>
       <c r="F49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H49" t="s">
         <v>110</v>
       </c>
       <c r="I49" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>45023</v>
+        <v>45030</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C50" s="5"/>
+        <v>169</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="E50" s="1"/>
       <c r="F50" t="s">
         <v>5</v>
-      </c>
-      <c r="G50" t="s">
-        <v>126</v>
       </c>
       <c r="H50" t="s">
         <v>110</v>
       </c>
+      <c r="I50" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>45018</v>
+        <v>45023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="F51" t="s">
         <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>126</v>
       </c>
       <c r="H51" t="s">
         <v>110</v>
@@ -5545,10 +5553,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>45017</v>
+        <v>45018</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="7"/>
@@ -5556,19 +5564,16 @@
       <c r="F52" t="s">
         <v>5</v>
       </c>
-      <c r="G52" t="s">
-        <v>126</v>
-      </c>
       <c r="H52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <v>45011</v>
+        <v>45017</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="7"/>
@@ -5576,16 +5581,19 @@
       <c r="F53" t="s">
         <v>5</v>
       </c>
+      <c r="G53" t="s">
+        <v>126</v>
+      </c>
       <c r="H53" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>45010</v>
+        <v>45011</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="7"/>
@@ -5593,68 +5601,63 @@
       <c r="F54" t="s">
         <v>5</v>
       </c>
-      <c r="G54" t="s">
-        <v>126</v>
-      </c>
       <c r="H54" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>45009</v>
+        <v>45010</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C55" s="5"/>
       <c r="D55" s="7"/>
       <c r="E55" s="1"/>
       <c r="F55" t="s">
         <v>5</v>
       </c>
+      <c r="G55" t="s">
+        <v>126</v>
+      </c>
       <c r="H55" t="s">
         <v>110</v>
       </c>
-      <c r="I55" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>45008</v>
+        <v>45009</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="D56" s="7"/>
-      <c r="E56" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" t="s">
         <v>5</v>
       </c>
       <c r="H56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I56" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <v>45005</v>
+        <v>45008</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="7"/>
       <c r="E57" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F57" t="s">
         <v>5</v>
@@ -5662,21 +5665,24 @@
       <c r="H57" t="s">
         <v>111</v>
       </c>
+      <c r="I57" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>45004</v>
+        <v>45005</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C58" s="5"/>
-      <c r="D58" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="1"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="F58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H58" t="s">
         <v>111</v>
@@ -5684,81 +5690,81 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <v>45001</v>
+        <v>45004</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" s="7"/>
+        <v>148</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="F59" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>44987</v>
+        <v>45001</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="1"/>
       <c r="F60" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H60" t="s">
-        <v>113</v>
-      </c>
-      <c r="I60" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <v>44982</v>
+        <v>44987</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="D61" s="7"/>
-      <c r="E61" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="E61" s="1"/>
       <c r="F61" t="s">
         <v>5</v>
       </c>
-      <c r="G61" t="s">
-        <v>126</v>
-      </c>
       <c r="H61" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="I61" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>44973</v>
+        <v>44982</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>145</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C62" s="5"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="F62" t="s">
-        <v>220</v>
+        <v>5</v>
+      </c>
+      <c r="G62" t="s">
+        <v>126</v>
       </c>
       <c r="H62" t="s">
         <v>111</v>
@@ -5766,32 +5772,29 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <v>44962</v>
+        <v>44973</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C63" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="D63" s="7"/>
-      <c r="E63" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="E63" s="1"/>
       <c r="F63" t="s">
-        <v>5</v>
-      </c>
-      <c r="G63" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="H63" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>44961</v>
+        <v>44962</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="7"/>
@@ -5810,29 +5813,32 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>44959</v>
+        <v>44961</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C65" s="5"/>
-      <c r="D65" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E65" s="1"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="F65" t="s">
         <v>5</v>
       </c>
+      <c r="G65" t="s">
+        <v>126</v>
+      </c>
       <c r="H65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>44955</v>
+        <v>44959</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="7" t="s">
@@ -5840,67 +5846,64 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>44947</v>
+        <v>44955</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="D67" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="1"/>
       <c r="F67" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H67" t="s">
-        <v>111</v>
-      </c>
-      <c r="I67" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>44945</v>
+        <v>44947</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C68" s="5"/>
-      <c r="D68" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E68" s="1"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="F68" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I68" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <v>44943</v>
+        <v>44945</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" t="s">
         <v>4</v>
@@ -5909,12 +5912,12 @@
         <v>110</v>
       </c>
       <c r="I69" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>13</v>
@@ -5936,52 +5939,52 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <v>44939</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>44942</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="1"/>
       <c r="F71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G71" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="H71" t="s">
         <v>110</v>
       </c>
+      <c r="I71" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>44937</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="1"/>
+        <v>44939</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F72" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G72" t="s">
+        <v>126</v>
       </c>
       <c r="H72" t="s">
-        <v>111</v>
-      </c>
-      <c r="I72" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
-        <v>44932</v>
+        <v>44937</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="1"/>
@@ -5997,38 +6000,38 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
-        <v>44930</v>
-      </c>
-      <c r="B74" s="1"/>
+        <v>44932</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C74" s="5" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="1"/>
       <c r="F74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H74" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="I74" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
-        <v>44928</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75" s="5"/>
+        <v>44930</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D75" s="7"/>
-      <c r="E75" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E75" s="1"/>
       <c r="F75" t="s">
         <v>5</v>
-      </c>
-      <c r="G75" t="s">
-        <v>126</v>
       </c>
       <c r="H75" t="s">
         <v>110</v>
@@ -6036,70 +6039,73 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
-        <v>44924</v>
+        <v>44928</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C76" s="5"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="1"/>
+      <c r="E76" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F76" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>126</v>
       </c>
       <c r="H76" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
-        <v>44922</v>
+        <v>44924</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C77" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="D77" s="7"/>
-      <c r="E77" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E77" s="1"/>
       <c r="F77" t="s">
-        <v>5</v>
-      </c>
-      <c r="G77" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H77" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
-        <v>44920</v>
+        <v>44922</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C78" s="5"/>
-      <c r="D78" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E78" s="1"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F78" t="s">
-        <v>220</v>
+        <v>5</v>
+      </c>
+      <c r="G78" t="s">
+        <v>126</v>
       </c>
       <c r="H78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
-        <v>44918</v>
+        <v>44920</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="7" t="s">
@@ -6107,43 +6113,43 @@
       </c>
       <c r="E79" s="1"/>
       <c r="F79" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="H79" t="s">
-        <v>114</v>
-      </c>
-      <c r="I79" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
-        <v>44912</v>
+        <v>44918</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E80" s="1"/>
       <c r="F80" t="s">
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="I80" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
-        <v>44903</v>
+        <v>44912</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="1"/>
@@ -6151,59 +6157,56 @@
         <v>5</v>
       </c>
       <c r="H81" t="s">
-        <v>114</v>
-      </c>
-      <c r="I81" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
-        <v>44896</v>
+        <v>44903</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" s="7"/>
       <c r="E82" s="1"/>
       <c r="F82" t="s">
         <v>5</v>
       </c>
       <c r="H82" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="I82" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
-        <v>44879</v>
+        <v>44896</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D83" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E83" s="1"/>
       <c r="F83" t="s">
         <v>5</v>
       </c>
-      <c r="G83" t="s">
-        <v>126</v>
-      </c>
       <c r="H83" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>44878</v>
+        <v>44879</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="7"/>
@@ -6222,10 +6225,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
-        <v>44877</v>
+        <v>44878</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="7"/>
@@ -6244,10 +6247,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
-        <v>44869</v>
+        <v>44877</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="7"/>
@@ -6257,46 +6260,49 @@
       <c r="F86" t="s">
         <v>5</v>
       </c>
+      <c r="G86" t="s">
+        <v>126</v>
+      </c>
       <c r="H86" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
-        <v>44864</v>
+        <v>44869</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="7"/>
       <c r="E87" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F87" t="s">
         <v>5</v>
       </c>
-      <c r="G87" t="s">
-        <v>126</v>
-      </c>
       <c r="H87" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
-        <v>44858</v>
+        <v>44864</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C88" s="5"/>
-      <c r="D88" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E88" s="1"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F88" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G88" t="s">
+        <v>126</v>
       </c>
       <c r="H88" t="s">
         <v>111</v>
@@ -6304,167 +6310,167 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
-        <v>44856</v>
+        <v>44858</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C89" s="5"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="D89" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E89" s="1"/>
       <c r="F89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H89" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
-        <v>44855</v>
-      </c>
-      <c r="B90" s="1"/>
+        <v>44856</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C90" s="5"/>
       <c r="D90" s="7"/>
       <c r="E90" s="1" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="F90" t="s">
         <v>5</v>
       </c>
-      <c r="G90" t="s">
-        <v>126</v>
-      </c>
       <c r="H90" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
-        <v>44850</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>44855</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="5"/>
       <c r="D91" s="7"/>
-      <c r="E91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F91" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="G91" t="s">
+        <v>126</v>
       </c>
       <c r="H91" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
-        <v>44845</v>
+        <v>44850</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="1"/>
       <c r="F92" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
-        <v>44843</v>
+        <v>44845</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C93" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="D93" s="7"/>
-      <c r="E93" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E93" s="1"/>
       <c r="F93" t="s">
-        <v>5</v>
-      </c>
-      <c r="G93" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="H93" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
-        <v>44840</v>
+        <v>44843</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C94" s="5"/>
       <c r="D94" s="7"/>
-      <c r="E94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F94" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G94" t="s">
+        <v>126</v>
       </c>
       <c r="H94" t="s">
         <v>111</v>
       </c>
-      <c r="I94" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
-        <v>44836</v>
-      </c>
-      <c r="B95" s="1"/>
-      <c r="C95" s="5"/>
+        <v>44840</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D95" s="7"/>
-      <c r="E95" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="E95" s="1"/>
       <c r="F95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H95" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="I95" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
-        <v>44834</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>44836</v>
+      </c>
+      <c r="B96" s="1"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E96" s="1"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F96" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="H96" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
-        <v>44833</v>
+        <v>44834</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="7" t="s">
@@ -6472,18 +6478,18 @@
       </c>
       <c r="E97" s="1"/>
       <c r="F97" t="s">
-        <v>6</v>
+        <v>220</v>
       </c>
       <c r="H97" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
-        <v>44831</v>
+        <v>44833</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="7" t="s">
@@ -6494,32 +6500,31 @@
         <v>6</v>
       </c>
       <c r="H98" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
-        <v>44827</v>
-      </c>
-      <c r="B99" s="1"/>
+        <v>44831</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C99" s="5"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D99" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E99" s="1"/>
       <c r="F99" t="s">
-        <v>5</v>
-      </c>
-      <c r="G99" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H99" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
-        <v>44826</v>
+        <v>44827</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="5"/>
@@ -6539,29 +6544,30 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
-        <v>44825</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>44826</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="5"/>
       <c r="D101" s="7"/>
-      <c r="E101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F101" t="s">
         <v>5</v>
       </c>
+      <c r="G101" t="s">
+        <v>126</v>
+      </c>
       <c r="H101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
-        <v>44824</v>
+        <v>44825</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>37</v>
@@ -6572,18 +6578,15 @@
         <v>5</v>
       </c>
       <c r="H102" t="s">
-        <v>110</v>
-      </c>
-      <c r="I102" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
-        <v>44823</v>
+        <v>44824</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>37</v>
@@ -6597,46 +6600,48 @@
         <v>110</v>
       </c>
       <c r="I103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
-        <v>44822</v>
+        <v>44823</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C104" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="D104" s="7"/>
       <c r="E104" s="1"/>
       <c r="F104" t="s">
-        <v>8</v>
-      </c>
-      <c r="G104" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H104" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="I104" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
-        <v>44821</v>
-      </c>
-      <c r="B105" s="1"/>
+        <v>44822</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C105" s="5"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="D105" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E105" s="1"/>
       <c r="F105" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G105" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H105" t="s">
         <v>111</v>
@@ -6644,13 +6649,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
-        <v>44815</v>
+        <v>44821</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="5"/>
       <c r="D106" s="7"/>
       <c r="E106" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F106" t="s">
         <v>5</v>
@@ -6664,13 +6669,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
-        <v>44814</v>
+        <v>44815</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="5"/>
       <c r="D107" s="7"/>
       <c r="E107" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F107" t="s">
         <v>5</v>
@@ -6679,21 +6684,19 @@
         <v>126</v>
       </c>
       <c r="H107" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
-        <v>44808</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>44814</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="5"/>
       <c r="D108" s="7"/>
-      <c r="E108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F108" t="s">
         <v>5</v>
       </c>
@@ -6701,152 +6704,154 @@
         <v>126</v>
       </c>
       <c r="H108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
-        <v>44801</v>
+        <v>44808</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="D109" s="7"/>
       <c r="E109" s="1"/>
       <c r="F109" t="s">
-        <v>220</v>
+        <v>5</v>
+      </c>
+      <c r="G109" t="s">
+        <v>126</v>
       </c>
       <c r="H109" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
-        <v>44793</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>44801</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E110" s="1"/>
       <c r="F110" t="s">
-        <v>5</v>
-      </c>
-      <c r="G110" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="H110" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
-        <v>44790</v>
-      </c>
-      <c r="B111" s="1"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="7"/>
+        <v>44793</v>
+      </c>
       <c r="E111" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F111" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G111" t="s">
+        <v>126</v>
       </c>
       <c r="H111" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
-        <v>44784</v>
+        <v>44790</v>
       </c>
       <c r="B112" s="1"/>
-      <c r="C112" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="C112" s="5"/>
       <c r="D112" s="7"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G112" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H112" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
-        <v>44782</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>44784</v>
+      </c>
+      <c r="B113" s="1"/>
       <c r="C113" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="1"/>
       <c r="F113" t="s">
         <v>5</v>
       </c>
+      <c r="G113" t="s">
+        <v>126</v>
+      </c>
       <c r="H113" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
-        <v>44770</v>
+        <v>44782</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C114" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D114" s="7"/>
-      <c r="E114" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E114" s="1"/>
       <c r="F114" t="s">
-        <v>8</v>
-      </c>
-      <c r="G114" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H114" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
-        <v>44760</v>
-      </c>
-      <c r="B115" s="1"/>
+        <v>44770</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C115" s="5"/>
       <c r="D115" s="7"/>
       <c r="E115" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F115" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G115" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H115" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
-        <v>44758</v>
+        <v>44760</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="5"/>
       <c r="D116" s="7"/>
       <c r="E116" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F116" t="s">
         <v>5</v>
@@ -6860,13 +6865,13 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
-        <v>44753</v>
+        <v>44758</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="5"/>
       <c r="D117" s="7"/>
       <c r="E117" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F117" t="s">
         <v>5</v>
@@ -6875,20 +6880,18 @@
         <v>126</v>
       </c>
       <c r="H117" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
-        <v>44747</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>44753</v>
+      </c>
+      <c r="B118" s="1"/>
       <c r="C118" s="5"/>
       <c r="D118" s="7"/>
       <c r="E118" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F118" t="s">
         <v>5</v>
@@ -6897,14 +6900,16 @@
         <v>126</v>
       </c>
       <c r="H118" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
-        <v>44746</v>
-      </c>
-      <c r="B119" s="1"/>
+        <v>44747</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C119" s="5"/>
       <c r="D119" s="7"/>
       <c r="E119" s="1" t="s">
@@ -6917,12 +6922,12 @@
         <v>126</v>
       </c>
       <c r="H119" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
-        <v>44745</v>
+        <v>44746</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="5"/>
@@ -6942,59 +6947,60 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
-        <v>44740</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>44745</v>
+      </c>
+      <c r="B121" s="1"/>
       <c r="C121" s="5"/>
       <c r="D121" s="7"/>
       <c r="E121" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F121" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G121" t="s">
+        <v>126</v>
       </c>
       <c r="H121" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
-        <v>44738</v>
+        <v>44740</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C122" s="5"/>
       <c r="D122" s="7"/>
       <c r="E122" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F122" t="s">
-        <v>5</v>
-      </c>
-      <c r="G122" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H122" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>44734</v>
+        <v>44738</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C123" s="5"/>
-      <c r="D123" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E123" s="1"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F123" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G123" t="s">
+        <v>126</v>
       </c>
       <c r="H123" t="s">
         <v>111</v>
@@ -7002,56 +7008,53 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>44731</v>
+        <v>44734</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D124" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E124" s="1"/>
       <c r="F124" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H124" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>44728</v>
+        <v>44731</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C125" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D125" s="7"/>
-      <c r="E125" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E125" s="1"/>
       <c r="F125" t="s">
-        <v>5</v>
-      </c>
-      <c r="G125" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="H125" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>44727</v>
+        <v>44728</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="7"/>
       <c r="E126" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F126" t="s">
         <v>5</v>
@@ -7060,61 +7063,63 @@
         <v>126</v>
       </c>
       <c r="H126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>44713</v>
+        <v>44727</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E127" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F127" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G127" t="s">
+        <v>126</v>
       </c>
       <c r="H127" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>44709</v>
+        <v>44713</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C128" s="5"/>
-      <c r="D128" s="7"/>
-      <c r="E128" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E128" s="1"/>
       <c r="F128" t="s">
-        <v>5</v>
-      </c>
-      <c r="G128" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="H128" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>44705</v>
-      </c>
-      <c r="B129" s="1"/>
+        <v>44709</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="C129" s="5"/>
       <c r="D129" s="7"/>
       <c r="E129" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F129" t="s">
         <v>5</v>
@@ -7123,173 +7128,173 @@
         <v>126</v>
       </c>
       <c r="H129" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
-        <v>44703</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>44705</v>
+      </c>
+      <c r="B130" s="1"/>
+      <c r="C130" s="5"/>
       <c r="D130" s="7"/>
-      <c r="E130" s="1"/>
+      <c r="E130" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F130" t="s">
         <v>5</v>
       </c>
+      <c r="G130" t="s">
+        <v>126</v>
+      </c>
       <c r="H130" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
-        <v>44702</v>
-      </c>
-      <c r="B131" s="1"/>
-      <c r="C131" s="5"/>
+        <v>44703</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="D131" s="7"/>
-      <c r="E131" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="E131" s="1"/>
       <c r="F131" t="s">
         <v>5</v>
       </c>
-      <c r="G131" t="s">
-        <v>126</v>
-      </c>
       <c r="H131" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
-        <v>44698</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>44702</v>
+      </c>
+      <c r="B132" s="1"/>
+      <c r="C132" s="5"/>
       <c r="D132" s="7"/>
-      <c r="E132" s="1"/>
+      <c r="E132" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F132" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G132" t="s">
+        <v>126</v>
       </c>
       <c r="H132" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
-        <v>44697</v>
+        <v>44698</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C133" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D133" s="7"/>
-      <c r="E133" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="E133" s="1"/>
       <c r="F133" t="s">
         <v>6</v>
       </c>
       <c r="H133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
-        <v>44693</v>
+        <v>44697</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C134" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C134" s="5"/>
       <c r="D134" s="7"/>
-      <c r="E134" s="1"/>
+      <c r="E134" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F134" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H134" t="s">
-        <v>110</v>
-      </c>
-      <c r="I134" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
-        <v>44689</v>
+        <v>44693</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D135" s="7"/>
       <c r="E135" s="1"/>
       <c r="F135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H135" t="s">
         <v>110</v>
       </c>
+      <c r="I135" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
-        <v>44686</v>
+        <v>44689</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="C136" s="5"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D136" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E136" s="1"/>
       <c r="F136" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H136" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
-        <v>44681</v>
+        <v>44686</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="C137" s="5"/>
       <c r="D137" s="7"/>
       <c r="E137" s="1" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="F137" t="s">
         <v>5</v>
       </c>
-      <c r="G137" t="s">
-        <v>126</v>
-      </c>
       <c r="H137" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
-        <v>44680</v>
-      </c>
-      <c r="B138" s="1"/>
+        <v>44681</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C138" s="5"/>
       <c r="D138" s="7"/>
       <c r="E138" s="1" t="s">
@@ -7307,198 +7312,199 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
-        <v>44664</v>
+        <v>44680</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="5"/>
       <c r="D139" s="7"/>
       <c r="E139" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F139" t="s">
         <v>5</v>
       </c>
+      <c r="G139" t="s">
+        <v>126</v>
+      </c>
       <c r="H139" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
-        <v>44653</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>44664</v>
+      </c>
+      <c r="B140" s="1"/>
       <c r="C140" s="5"/>
       <c r="D140" s="7"/>
       <c r="E140" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="F140" t="s">
         <v>5</v>
       </c>
       <c r="H140" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
-        <v>44650</v>
+        <v>44653</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C141" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C141" s="5"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="1"/>
+      <c r="E141" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F141" t="s">
         <v>5</v>
       </c>
       <c r="H141" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
-        <v>44647</v>
+        <v>44650</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C142" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D142" s="7"/>
-      <c r="E142" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="E142" s="1"/>
       <c r="F142" t="s">
         <v>5</v>
       </c>
       <c r="H142" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
-        <v>44630</v>
+        <v>44647</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C143" s="5"/>
-      <c r="D143" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E143" s="1"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F143" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H143" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
-        <v>44614</v>
+        <v>44630</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D144" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="C144" s="5"/>
+      <c r="D144" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E144" s="1"/>
       <c r="F144" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H144" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
-        <v>44604</v>
+        <v>44614</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C145" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D145" s="7"/>
-      <c r="E145" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E145" s="1"/>
       <c r="F145" t="s">
         <v>5</v>
       </c>
       <c r="H145" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
-        <v>44600</v>
+        <v>44604</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C146" s="5"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="1"/>
+      <c r="E146" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F146" t="s">
         <v>5</v>
       </c>
       <c r="H146" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
-        <v>44597</v>
+        <v>44600</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C147" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D147" s="7"/>
-      <c r="E147" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="E147" s="1"/>
       <c r="F147" t="s">
         <v>5</v>
       </c>
       <c r="H147" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
-        <v>44595</v>
+        <v>44597</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C148" s="5"/>
       <c r="D148" s="7"/>
       <c r="E148" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F148" t="s">
         <v>5</v>
       </c>
       <c r="H148" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
-        <v>44593</v>
+        <v>44595</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C149" s="5"/>
       <c r="D149" s="7"/>
@@ -7509,81 +7515,78 @@
         <v>5</v>
       </c>
       <c r="H149" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
-        <v>44590</v>
+        <v>44593</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="7"/>
       <c r="E150" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F150" t="s">
         <v>5</v>
       </c>
       <c r="H150" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
-        <v>44588</v>
+        <v>44590</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C151" s="5"/>
       <c r="D151" s="7"/>
       <c r="E151" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F151" t="s">
         <v>5</v>
       </c>
       <c r="H151" t="s">
-        <v>110</v>
-      </c>
-      <c r="I151" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
-        <v>44585</v>
+        <v>44588</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C152" s="5"/>
       <c r="D152" s="7"/>
-      <c r="E152" s="1"/>
+      <c r="E152" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F152" t="s">
         <v>5</v>
       </c>
       <c r="H152" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I152" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
-        <v>44582</v>
+        <v>44585</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="D153" s="7"/>
       <c r="E153" s="1"/>
@@ -7591,70 +7594,73 @@
         <v>5</v>
       </c>
       <c r="H153" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="I153" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
-        <v>44578</v>
-      </c>
-      <c r="B154" s="1"/>
-      <c r="C154" s="5"/>
+        <v>44582</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D154" s="7"/>
-      <c r="E154" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E154" s="1"/>
       <c r="F154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H154" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
-        <v>44576</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>44578</v>
+      </c>
+      <c r="B155" s="1"/>
       <c r="C155" s="5"/>
       <c r="D155" s="7"/>
       <c r="E155" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F155" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H155" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
-        <v>44575</v>
+        <v>44576</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="7"/>
       <c r="E156" s="1" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="F156" t="s">
         <v>5</v>
       </c>
       <c r="H156" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
-        <v>44567</v>
+        <v>44575</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C157" s="5"/>
       <c r="D157" s="7"/>
@@ -7662,10 +7668,7 @@
         <v>85</v>
       </c>
       <c r="F157" t="s">
-        <v>9</v>
-      </c>
-      <c r="G157" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H157" t="s">
         <v>110</v>
@@ -7673,18 +7676,21 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
-        <v>44564</v>
+        <v>44567</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C158" s="5"/>
       <c r="D158" s="7"/>
-      <c r="E158" s="1"/>
+      <c r="E158" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="F158" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="G158" t="s">
+        <v>121</v>
       </c>
       <c r="H158" t="s">
         <v>110</v>
@@ -7692,13 +7698,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
-        <v>44558</v>
+        <v>44564</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="1"/>
@@ -7706,38 +7712,38 @@
         <v>5</v>
       </c>
       <c r="H159" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
-        <v>44532</v>
-      </c>
-      <c r="B160" s="1"/>
-      <c r="C160" s="5"/>
+        <v>44558</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D160" s="7"/>
-      <c r="E160" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="E160" s="1"/>
       <c r="F160" t="s">
         <v>5</v>
       </c>
       <c r="H160" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
-        <v>44526</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>44532</v>
+      </c>
+      <c r="B161" s="1"/>
+      <c r="C161" s="5"/>
       <c r="D161" s="7"/>
-      <c r="E161" s="1"/>
+      <c r="E161" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="F161" t="s">
         <v>5</v>
       </c>
@@ -7747,109 +7753,109 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
-        <v>44519</v>
+        <v>44526</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D162" s="7"/>
       <c r="E162" s="1"/>
       <c r="F162" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H162" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
-        <v>44507</v>
-      </c>
-      <c r="B163" s="1"/>
+        <v>44519</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="C163" s="5"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="D163" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E163" s="1"/>
       <c r="F163" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H163" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
-        <v>44495</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>44507</v>
+      </c>
+      <c r="B164" s="1"/>
+      <c r="C164" s="5"/>
       <c r="D164" s="7"/>
-      <c r="E164" s="1"/>
+      <c r="E164" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F164" t="s">
-        <v>9</v>
-      </c>
-      <c r="G164" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H164" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
-        <v>44487</v>
+        <v>44495</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C165" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D165" s="7"/>
-      <c r="E165" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E165" s="1"/>
       <c r="F165" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="G165" t="s">
+        <v>121</v>
       </c>
       <c r="H165" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
-        <v>44471</v>
+        <v>44487</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C166" s="5"/>
       <c r="D166" s="7"/>
-      <c r="E166" s="1"/>
+      <c r="E166" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F166" t="s">
         <v>5</v>
       </c>
       <c r="H166" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
-        <v>44462</v>
+        <v>44471</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="D167" s="7"/>
       <c r="E167" s="1"/>
@@ -7857,65 +7863,62 @@
         <v>5</v>
       </c>
       <c r="H167" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
-        <v>44446</v>
+        <v>44462</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C168" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D168" s="7"/>
-      <c r="E168" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E168" s="1"/>
       <c r="F168" t="s">
         <v>5</v>
       </c>
       <c r="H168" t="s">
         <v>111</v>
       </c>
-      <c r="I168" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
-        <v>44445</v>
+        <v>44446</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C169" s="5"/>
       <c r="D169" s="7"/>
-      <c r="E169" s="1"/>
+      <c r="E169" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F169" t="s">
-        <v>9</v>
-      </c>
-      <c r="G169" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="H169" t="s">
         <v>111</v>
       </c>
+      <c r="I169" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
-        <v>44440</v>
+        <v>44445</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C170" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D170" s="7"/>
-      <c r="E170" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E170" s="1"/>
       <c r="F170" t="s">
         <v>9</v>
       </c>
@@ -7928,15 +7931,15 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
-        <v>44418</v>
+        <v>44440</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C171" s="5"/>
       <c r="D171" s="7"/>
       <c r="E171" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F171" t="s">
         <v>9</v>
@@ -7950,10 +7953,10 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
-        <v>44417</v>
+        <v>44418</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C172" s="5"/>
       <c r="D172" s="7"/>
@@ -7967,12 +7970,34 @@
         <v>121</v>
       </c>
       <c r="H172" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>44417</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C173" s="5"/>
+      <c r="D173" s="7"/>
+      <c r="E173" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F173" t="s">
+        <v>9</v>
+      </c>
+      <c r="G173" t="s">
+        <v>121</v>
+      </c>
+      <c r="H173" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D136 D138:D1048576">
+  <conditionalFormatting sqref="D1:D137 D139:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>